<commit_message>
factor out portfolio handls
</commit_message>
<xml_diff>
--- a/excel/test.xlsx
+++ b/excel/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1009dev\source\repos\xlladdins\xll_allocation\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93382FA9-E995-45F9-AF27-9B75BBD7C3B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC8C5D5-98C1-4917-B12B-FC8BBD028823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C1522A91-786E-4C1B-8BA2-06271DEDE1ED}"/>
   </bookViews>
@@ -16,10 +16,15 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="Cov">Sheet1!$C$3:$E$5</definedName>
     <definedName name="ER">Sheet1!$C$2:$E$2</definedName>
-    <definedName name="sigma">Sheet1!$C$6</definedName>
-    <definedName name="V">Sheet1!$C$3:$E$5</definedName>
-    <definedName name="weight">Sheet1!$C$8:$E$8</definedName>
+    <definedName name="lower">Sheet1!$C$7:$G$7</definedName>
+    <definedName name="portfolio">Sheet1!$C$6</definedName>
+    <definedName name="R_">Sheet1!$C$10</definedName>
+    <definedName name="realized">Sheet1!#REF!</definedName>
+    <definedName name="sigma">Sheet1!$C$14</definedName>
+    <definedName name="upper">Sheet1!$C$8:$G$8</definedName>
+    <definedName name="weight">Sheet1!$C$15:$E$15</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +45,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -62,10 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>V</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>ER</t>
   </si>
@@ -73,20 +75,49 @@
     <t>sigma</t>
   </si>
   <si>
-    <t>weight</t>
-  </si>
-  <si>
     <t>lambda</t>
   </si>
   <si>
     <t>mu</t>
+  </si>
+  <si>
+    <t>portfolio</t>
+  </si>
+  <si>
+    <t>Cov</t>
+  </si>
+  <si>
+    <t>maximize</t>
+  </si>
+  <si>
+    <t>minimize</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>lower</t>
+  </si>
+  <si>
+    <t>upper</t>
+  </si>
+  <si>
+    <t>minimum</t>
+  </si>
+  <si>
+    <t>maximum</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0E+00"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,6 +147,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -135,7 +180,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -173,20 +218,122 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="2" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Input" xfId="1" builtinId="20"/>
@@ -506,717 +653,824 @@
   <dimension ref="B1:W21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="3" max="7" width="9.140625" customWidth="1"/>
     <col min="21" max="21" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:23" x14ac:dyDescent="0.25">
       <c r="U1">
-        <f>AVERAGE(Q2:Q21)</f>
-        <v>0.4176589472860896</v>
+        <f>AVERAGE(Q2:Q21)-U2</f>
+        <v>0</v>
       </c>
       <c r="V1">
-        <f>AVERAGE(R2:R21)</f>
-        <v>0.58112987806403582</v>
+        <f>AVERAGE(R2:R21)-V2</f>
+        <v>0</v>
       </c>
       <c r="W1">
-        <f>AVERAGE(S2:S21)</f>
-        <v>0.43984539065022232</v>
+        <f>AVERAGE(S2:S21)-W2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2">
-        <v>0.41765894728608965</v>
-      </c>
-      <c r="D2" s="2">
-        <v>0.58112987806403593</v>
-      </c>
-      <c r="E2" s="2">
-        <v>0.43984539065022232</v>
+        <v>0</v>
+      </c>
+      <c r="C2" s="5">
+        <f>U2</f>
+        <v>1.5384667499736222</v>
+      </c>
+      <c r="D2" s="5">
+        <f t="shared" ref="D2:D5" si="0">V2</f>
+        <v>1.5002363144118562</v>
+      </c>
+      <c r="E2" s="5">
+        <f t="shared" ref="E2:E5" si="1">W2</f>
+        <v>1.4399328500861042</v>
       </c>
       <c r="I2">
-        <f ca="1">RAND()</f>
-        <v>0.86487471005461047</v>
+        <f ca="1">1+RAND()</f>
+        <v>1.2515519641560882</v>
       </c>
       <c r="J2">
-        <f t="shared" ref="J2:K21" ca="1" si="0">RAND()</f>
-        <v>0.36605327740363147</v>
+        <f t="shared" ref="J2:K21" ca="1" si="2">1+RAND()</f>
+        <v>1.4509108495327752</v>
       </c>
       <c r="K2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.57928605675696532</v>
-      </c>
-      <c r="M2" cm="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>1.5881336184052435</v>
+      </c>
+      <c r="M2" s="12" cm="1">
         <f t="array" aca="1" ref="M2:O5" ca="1">_xll.AFBI.COV(I2:K21)</f>
-        <v>0.52373014035637599</v>
-      </c>
-      <c r="N2">
+        <v>1.4730727883134191</v>
+      </c>
+      <c r="N2" s="12">
         <f ca="1"/>
-        <v>0.51155150138964567</v>
-      </c>
-      <c r="O2">
+        <v>1.4990664739415369</v>
+      </c>
+      <c r="O2" s="12">
         <f ca="1"/>
-        <v>0.53496195501663957</v>
+        <v>1.4539196142742736</v>
       </c>
       <c r="Q2">
-        <v>0.63059339319181351</v>
+        <v>1.6724228739076512</v>
       </c>
       <c r="R2">
-        <v>0.99418612484505586</v>
+        <v>1.832624962280506</v>
       </c>
       <c r="S2">
-        <v>0.79382771852181766</v>
-      </c>
-      <c r="U2">
-        <v>0.41765894728608965</v>
+        <v>1.3503434013490421</v>
+      </c>
+      <c r="U2" cm="1">
+        <f t="array" ref="U2:W5">_xll.AFBI.COV(Q2:S21)</f>
+        <v>1.5384667499736222</v>
       </c>
       <c r="V2">
-        <v>0.58112987806403593</v>
+        <v>1.5002363144118562</v>
       </c>
       <c r="W2">
-        <v>0.43984539065022232</v>
+        <v>1.4399328500861042</v>
       </c>
     </row>
     <row r="3" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0.10109818608804175</v>
-      </c>
-      <c r="D3" s="2">
-        <v>2.6080292198810862E-2</v>
-      </c>
-      <c r="E3" s="2">
-        <v>2.8770843267289431E-2</v>
+        <v>5</v>
+      </c>
+      <c r="C3" s="5">
+        <f t="shared" ref="C3:C5" si="3">U3</f>
+        <v>8.8964336185242132E-2</v>
+      </c>
+      <c r="D3" s="5">
+        <f t="shared" si="0"/>
+        <v>2.5648208896523084E-2</v>
+      </c>
+      <c r="E3" s="5">
+        <f t="shared" si="1"/>
+        <v>-4.5409549415085237E-3</v>
+      </c>
+      <c r="F3">
+        <f>SQRT(C3)</f>
+        <v>0.29826889912500454</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I21" ca="1" si="1">RAND()</f>
-        <v>0.11540921116763536</v>
+        <f t="shared" ref="I3:I21" ca="1" si="4">1+RAND()</f>
+        <v>1.869393652474034</v>
       </c>
       <c r="J3">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.12040340771246771</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1.5918178627603892</v>
       </c>
       <c r="K3">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.88426923394848811</v>
-      </c>
-      <c r="M3">
+        <f t="shared" ca="1" si="2"/>
+        <v>1.0471462511659229</v>
+      </c>
+      <c r="M3" s="13">
         <f ca="1"/>
-        <v>9.692602667321909E-2</v>
-      </c>
-      <c r="N3">
+        <v>8.9416790656735579E-2</v>
+      </c>
+      <c r="N3" s="14">
         <f ca="1"/>
-        <v>3.3895221316900259E-3</v>
-      </c>
-      <c r="O3">
+        <v>-3.650252548914823E-2</v>
+      </c>
+      <c r="O3" s="15">
         <f ca="1"/>
-        <v>-5.0409666808805542E-3</v>
+        <v>-3.1689484116773414E-2</v>
       </c>
       <c r="Q3">
-        <v>6.6506966651322608E-2</v>
+        <v>1.0999296210412119</v>
       </c>
       <c r="R3">
-        <v>7.5478746044538303E-2</v>
+        <v>1.6614823281862048</v>
       </c>
       <c r="S3">
-        <v>0.45471622727443173</v>
-      </c>
-      <c r="U3">
-        <v>0.10109818608804175</v>
-      </c>
-      <c r="V3">
-        <v>2.6080292198810862E-2</v>
-      </c>
-      <c r="W3">
-        <v>2.8770843267289431E-2</v>
+        <v>1.3334043183880735</v>
+      </c>
+      <c r="U3" s="13">
+        <v>8.8964336185242132E-2</v>
+      </c>
+      <c r="V3" s="14">
+        <v>2.5648208896523084E-2</v>
+      </c>
+      <c r="W3" s="15">
+        <v>-4.5409549415085237E-3</v>
       </c>
     </row>
     <row r="4" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C4" s="2">
-        <v>2.6080292198810862E-2</v>
-      </c>
-      <c r="D4" s="2">
-        <v>6.3881424579278423E-2</v>
-      </c>
-      <c r="E4" s="2">
-        <v>-6.6703847854753529E-3</v>
+      <c r="C4" s="5">
+        <f t="shared" si="3"/>
+        <v>2.5648208896523084E-2</v>
+      </c>
+      <c r="D4" s="5">
+        <f t="shared" si="0"/>
+        <v>0.10048451058259911</v>
+      </c>
+      <c r="E4" s="5">
+        <f t="shared" si="1"/>
+        <v>1.8021338123195285E-3</v>
       </c>
       <c r="I4">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.79190136451919546</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>1.2371885053201277</v>
       </c>
       <c r="J4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.43560354869853923</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1.9263740234804103</v>
       </c>
       <c r="K4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.7023447691451461</v>
-      </c>
-      <c r="M4">
+        <f t="shared" ca="1" si="2"/>
+        <v>1.6985111057602478</v>
+      </c>
+      <c r="M4" s="16">
         <f ca="1"/>
-        <v>3.3895221316900259E-3</v>
-      </c>
-      <c r="N4">
+        <v>-3.650252548914823E-2</v>
+      </c>
+      <c r="N4" s="17">
         <f ca="1"/>
-        <v>5.3760783472370621E-2</v>
-      </c>
-      <c r="O4">
+        <v>6.859345119450877E-2</v>
+      </c>
+      <c r="O4" s="18">
         <f ca="1"/>
-        <v>-1.9187275892076361E-3</v>
+        <v>-3.5239991090780798E-3</v>
       </c>
       <c r="Q4">
-        <v>0.77204045514424791</v>
+        <v>1.4390575770759571</v>
       </c>
       <c r="R4">
-        <v>0.35214863788661754</v>
+        <v>1.6423380868210862</v>
       </c>
       <c r="S4">
-        <v>0.64903756720856665</v>
-      </c>
-      <c r="U4">
-        <v>2.6080292198810862E-2</v>
-      </c>
-      <c r="V4">
-        <v>6.3881424579278423E-2</v>
-      </c>
-      <c r="W4">
-        <v>-6.6703847854753529E-3</v>
+        <v>1.3785889173831487</v>
+      </c>
+      <c r="U4" s="16">
+        <v>2.5648208896523084E-2</v>
+      </c>
+      <c r="V4" s="17">
+        <v>0.10048451058259911</v>
+      </c>
+      <c r="W4" s="18">
+        <v>1.8021338123195285E-3</v>
       </c>
     </row>
     <row r="5" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C5" s="2">
-        <v>2.8770843267289431E-2</v>
-      </c>
-      <c r="D5" s="2">
-        <v>-6.6703847854753529E-3</v>
-      </c>
-      <c r="E5" s="2">
-        <v>7.5057875342522506E-2</v>
+      <c r="C5" s="5">
+        <f t="shared" si="3"/>
+        <v>-4.5409549415085237E-3</v>
+      </c>
+      <c r="D5" s="5">
+        <f t="shared" si="0"/>
+        <v>1.8021338123195285E-3</v>
+      </c>
+      <c r="E5" s="5">
+        <f t="shared" si="1"/>
+        <v>8.9597339814333488E-2</v>
       </c>
       <c r="I5">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.98272090242343579</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>1.9234280844635099</v>
       </c>
       <c r="J5">
-        <f t="shared" ca="1" si="0"/>
-        <v>8.2628236273149747E-2</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1.3969846673469326</v>
       </c>
       <c r="K5">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.4585389464727867</v>
-      </c>
-      <c r="M5">
+        <f t="shared" ca="1" si="2"/>
+        <v>1.379117033554961</v>
+      </c>
+      <c r="M5" s="19">
         <f ca="1"/>
-        <v>-5.0409666808805542E-3</v>
-      </c>
-      <c r="N5">
+        <v>-3.1689484116773414E-2</v>
+      </c>
+      <c r="N5" s="12">
         <f ca="1"/>
-        <v>-1.9187275892076361E-3</v>
-      </c>
-      <c r="O5">
+        <v>-3.5239991090780798E-3</v>
+      </c>
+      <c r="O5" s="20">
         <f ca="1"/>
-        <v>5.0890628232860391E-2</v>
+        <v>8.3255955836111895E-2</v>
       </c>
       <c r="Q5">
-        <v>5.4762517115893528E-2</v>
+        <v>1.8696199837738985</v>
       </c>
       <c r="R5">
-        <v>0.7825307019878569</v>
+        <v>1.2190539553512734</v>
       </c>
       <c r="S5">
-        <v>0.68402443130079993</v>
-      </c>
-      <c r="U5">
-        <v>2.8770843267289431E-2</v>
-      </c>
-      <c r="V5">
-        <v>-6.6703847854753529E-3</v>
-      </c>
-      <c r="W5">
-        <v>7.5057875342522506E-2</v>
+        <v>1.0732773370049091</v>
+      </c>
+      <c r="U5" s="19">
+        <v>-4.5409549415085237E-3</v>
+      </c>
+      <c r="V5" s="12">
+        <v>1.8021338123195285E-3</v>
+      </c>
+      <c r="W5" s="20">
+        <v>8.9597339814333488E-2</v>
       </c>
     </row>
     <row r="6" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4" cm="1">
+        <f t="array" ref="C6">_xll.\AFBI.ALLOCATION(ER, Cov)</f>
+        <v>2326360968624</v>
+      </c>
+      <c r="F6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="2">
-        <v>0.1</v>
+      <c r="G6" s="9" t="s">
+        <v>3</v>
       </c>
       <c r="I6">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.30306720236745222</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>1.4416692628071441</v>
       </c>
       <c r="J6">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.43436028781650893</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1.0997575655561631</v>
       </c>
       <c r="K6">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.87466570005550714</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1.9269821794457807</v>
       </c>
       <c r="Q6">
-        <v>0.98224921677346688</v>
+        <v>1.8349353619490156</v>
       </c>
       <c r="R6">
-        <v>0.74305878367105904</v>
+        <v>1.7742836872271723</v>
       </c>
       <c r="S6">
-        <v>0.69335829741327848</v>
+        <v>1.839707427135119</v>
       </c>
     </row>
     <row r="7" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="F7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G7" t="s">
-        <v>5</v>
+      <c r="B7" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0</v>
+      </c>
+      <c r="F7" s="10" cm="1">
+        <f t="array" ref="F7">-_xll.DBL_MAX()</f>
+        <v>-1.7976931348623157E+308</v>
+      </c>
+      <c r="G7" s="10" cm="1">
+        <f t="array" ref="G7">-_xll.DBL_MAX()</f>
+        <v>-1.7976931348623157E+308</v>
       </c>
       <c r="I7">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.90622341463075085</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>1.5113478059673049</v>
       </c>
       <c r="J7">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.63974228493036711</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1.5535048358394339</v>
       </c>
       <c r="K7">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.29515968830172712</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1.2245806991157648</v>
+      </c>
+      <c r="N7" t="b">
+        <f ca="1">N3=M4</f>
+        <v>1</v>
+      </c>
+      <c r="O7" t="b">
+        <f ca="1">O3=M5</f>
+        <v>1</v>
       </c>
       <c r="Q7">
-        <v>0.84036124969205661</v>
+        <v>1.3163306402517865</v>
       </c>
       <c r="R7">
-        <v>0.40558099164380146</v>
+        <v>1.4165686671792466</v>
       </c>
       <c r="S7">
-        <v>0.94635843118370488</v>
+        <v>1.8568942440363156</v>
       </c>
       <c r="U7">
         <f>COVAR(Q2:Q21,Q2:Q21)</f>
-        <v>0.10109818608804164</v>
+        <v>8.8964336185242424E-2</v>
       </c>
       <c r="V7">
         <f>COVAR(Q2:Q21,R2:R21)</f>
-        <v>2.6080292198810896E-2</v>
+        <v>2.5648208896523271E-2</v>
       </c>
       <c r="W7">
         <f>COVAR(Q2:Q21,S2:S21)</f>
-        <v>2.8770843267289386E-2</v>
+        <v>-4.5409549415086087E-3</v>
       </c>
     </row>
     <row r="8" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="3" cm="1">
-        <f t="array" ref="C8:G8">_xll.AFBI.ALLOCATION.MAXIMIZE(ER, V, sigma, 0)</f>
-        <v>0.27612619627659218</v>
-      </c>
-      <c r="D8" s="3">
-        <v>0.41120608284679078</v>
-      </c>
-      <c r="E8" s="3">
-        <v>0.31266772087661715</v>
-      </c>
-      <c r="F8" s="4">
-        <v>-0.40398508344492257</v>
-      </c>
-      <c r="G8" s="4">
-        <v>29.432878016550227</v>
+      <c r="B8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="2" cm="1">
+        <f t="array" ref="C8">_xll.DBL_MAX()</f>
+        <v>1.7976931348623157E+308</v>
+      </c>
+      <c r="D8" s="2" cm="1">
+        <f t="array" ref="D8">_xll.DBL_MAX()</f>
+        <v>1.7976931348623157E+308</v>
+      </c>
+      <c r="E8" s="2" cm="1">
+        <f t="array" ref="E8">_xll.DBL_MAX()</f>
+        <v>1.7976931348623157E+308</v>
+      </c>
+      <c r="F8" s="2" cm="1">
+        <f t="array" ref="F8">_xll.DBL_MAX()</f>
+        <v>1.7976931348623157E+308</v>
+      </c>
+      <c r="G8" s="2" cm="1">
+        <f t="array" ref="G8">_xll.DBL_MAX()</f>
+        <v>1.7976931348623157E+308</v>
       </c>
       <c r="I8">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.61752315717792772</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>1.6369871838548611</v>
       </c>
       <c r="J8">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.33170934422280618</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1.5813858740180105</v>
       </c>
       <c r="K8">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.23689970932184901</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1.0608325647168277</v>
+      </c>
+      <c r="O8" t="b">
+        <f ca="1">O4=N5</f>
+        <v>1</v>
       </c>
       <c r="Q8">
-        <v>0.11574532256328796</v>
+        <v>1.2541869167279776</v>
       </c>
       <c r="R8">
-        <v>0.74022752026688832</v>
+        <v>1.094780111107712</v>
       </c>
       <c r="S8">
-        <v>0.54150749080004934</v>
+        <v>1.2787058521270982</v>
       </c>
       <c r="V8">
         <f>COVAR(R2:R21,R2:R21)</f>
-        <v>6.3881424579278395E-2</v>
+        <v>0.10048451058259991</v>
       </c>
       <c r="W8">
         <f>COVAR(R2:R21,S2:S21)</f>
-        <v>-6.6703847854753338E-3</v>
+        <v>1.8021338123198366E-3</v>
       </c>
     </row>
     <row r="9" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C9" cm="1">
-        <f t="array" ref="C9:D9">_xll.AFBI.ALLOCATION.INFO(ER, V, C8:E8)</f>
-        <v>0.49181617307162939</v>
-      </c>
-      <c r="D9">
-        <v>0.18714435747783109</v>
-      </c>
       <c r="I9">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.1248339274816499</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>1.0616072202264912</v>
       </c>
       <c r="J9">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.66183884578049412</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1.2992708257527261</v>
       </c>
       <c r="K9">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.32303470144880764</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1.9840081535601546</v>
       </c>
       <c r="Q9">
-        <v>4.7157028160988657E-2</v>
+        <v>1.3278353737671185</v>
       </c>
       <c r="R9">
-        <v>0.48623932033483119</v>
+        <v>1.1030235396756756</v>
       </c>
       <c r="S9">
-        <v>0.30210948316783359</v>
+        <v>1.9835107346557226</v>
       </c>
       <c r="W9">
         <f>COVAR(S2:S21,S2:S21)</f>
-        <v>7.5057875342522534E-2</v>
+        <v>8.9597339814333737E-2</v>
       </c>
     </row>
     <row r="10" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C10">
-        <f>SUMPRODUCT(weight,ER)</f>
-        <v>0.49181617307162939</v>
-      </c>
-      <c r="D10" cm="1">
-        <f t="array" ref="D10">SQRT(MMULT(weight,MMULT(V,TRANSPOSE(weight))))</f>
-        <v>0.18714435747783109</v>
+      <c r="B10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="D10" s="21">
+        <f>SUMPRODUCT(C11:E11,ER)</f>
+        <v>1.4581487863039357</v>
       </c>
       <c r="I10">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.32244976044348794</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>1.3897496236130147</v>
       </c>
       <c r="J10">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.28413329657250508</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1.4714862893839884</v>
       </c>
       <c r="K10">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.17683741321187929</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1.7400119807125765</v>
       </c>
       <c r="Q10">
-        <v>0.74964701013081503</v>
+        <v>1.2285720898044827</v>
       </c>
       <c r="R10">
-        <v>0.67304375062875477</v>
+        <v>1.3480781337158216</v>
       </c>
       <c r="S10">
-        <v>0.2630594348442824</v>
+        <v>1.0699592800916942</v>
       </c>
     </row>
     <row r="11" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C11">
-        <f>C9-C10</f>
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <f>D9-D10</f>
-        <v>0</v>
+      <c r="B11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="6" cm="1">
+        <f t="array" ref="C11:G11">_xll.AFBI.ALLOCATION.MINIMIZE(portfolio, R_, 0)</f>
+        <v>2.7720340661606484E-2</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0.25677700476083176</v>
+      </c>
+      <c r="E11" s="6">
+        <v>0.71550265457753737</v>
+      </c>
+      <c r="F11" s="7">
+        <v>0.97016263566332517</v>
+      </c>
+      <c r="G11" s="7">
+        <v>-0.6290006033436395</v>
       </c>
       <c r="I11">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.92887684506076029</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>1.343009468397915</v>
       </c>
       <c r="J11">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.54385716508961701</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1.7356064579320023</v>
       </c>
       <c r="K11">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.92608308556912211</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1.413019290402127</v>
       </c>
       <c r="Q11">
-        <v>6.4903819947050856E-3</v>
+        <v>1.3684795590972687</v>
       </c>
       <c r="R11">
-        <v>0.21079890528500334</v>
+        <v>1.8208822026965081</v>
       </c>
       <c r="S11">
-        <v>0.44090267109886561</v>
+        <v>1.3497031974283589</v>
       </c>
       <c r="U11">
         <f>U3-U7</f>
-        <v>1.1102230246251565E-16</v>
+        <v>-2.9143354396410359E-16</v>
       </c>
       <c r="V11">
         <f>V3-V7</f>
-        <v>-3.4694469519536142E-17</v>
+        <v>-1.8735013540549517E-16</v>
       </c>
       <c r="W11">
         <f>W3-W7</f>
-        <v>4.5102810375396984E-17</v>
+        <v>8.5001450322863548E-17</v>
       </c>
     </row>
     <row r="12" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B12" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="6" cm="1">
+        <f t="array" ref="C12">_xll.AFBI.ALLOCATION.MINIMUM(portfolio, R_)</f>
+        <v>0.29926876045158723</v>
+      </c>
       <c r="I12">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.12475162969611586</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>1.1793482205886003</v>
       </c>
       <c r="J12">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.54511013231697836</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1.928901645530315</v>
       </c>
       <c r="K12">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.22038514244073026</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1.5149579307556136</v>
       </c>
       <c r="Q12">
-        <v>0.28824327747141476</v>
+        <v>1.2199462308238882</v>
       </c>
       <c r="R12">
-        <v>0.94190746978272344</v>
+        <v>1.7406951482664867</v>
       </c>
       <c r="S12">
-        <v>0.2445152067023173</v>
+        <v>1.2555387658700483</v>
       </c>
       <c r="V12">
         <f>V4-V8</f>
-        <v>0</v>
+        <v>-8.0491169285323849E-16</v>
       </c>
       <c r="W12">
         <f>W4-W8</f>
-        <v>-1.9081958235744878E-17</v>
+        <v>-3.0813025742038036E-16</v>
       </c>
     </row>
     <row r="13" spans="2:23" x14ac:dyDescent="0.25">
       <c r="I13">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.63181491167769277</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>1.7012777582817056</v>
       </c>
       <c r="J13">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.82403991608643767</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1.2742271485801546</v>
       </c>
       <c r="K13">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.43489320581270674</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1.0249552587668149</v>
       </c>
       <c r="Q13">
-        <v>0.18227771310028718</v>
+        <v>1.7151340649864826</v>
       </c>
       <c r="R13">
-        <v>0.52009388996737871</v>
+        <v>1.9773277051529012</v>
       </c>
       <c r="S13">
-        <v>1.2437536643746805E-3</v>
+        <v>1.9333912408748204</v>
       </c>
       <c r="W13">
         <f>W5-W9</f>
-        <v>0</v>
+        <v>-2.4980018054066022E-16</v>
       </c>
     </row>
     <row r="14" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="11">
+        <v>0.3</v>
+      </c>
+      <c r="D14" s="22">
+        <f>SUMPRODUCT(MMULT(ER,Cov),ER)</f>
+        <v>0.72856343914929411</v>
+      </c>
       <c r="I14">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.92634993225754458</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>1.1013157211111264</v>
       </c>
       <c r="J14">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.84864532255739111</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1.7099524477055468</v>
       </c>
       <c r="K14">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.3441925490408283</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1.2692248451753936</v>
       </c>
       <c r="Q14">
-        <v>0.2802067276708281</v>
+        <v>1.1151597871905503</v>
       </c>
       <c r="R14">
-        <v>0.80389765024280702</v>
+        <v>1.0412145161602686</v>
       </c>
       <c r="S14">
-        <v>0.13096457897042424</v>
+        <v>1.6359526472504462</v>
       </c>
     </row>
     <row r="15" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="6" cm="1">
+        <f t="array" ref="C15:G15">_xll.AFBI.ALLOCATION.MAXIMIZE(portfolio, sigma, 0)</f>
+        <v>0.72521836666867401</v>
+      </c>
+      <c r="D15" s="6">
+        <v>0.21672360817836653</v>
+      </c>
+      <c r="E15" s="6">
+        <v>5.8058025152956189E-2</v>
+      </c>
+      <c r="F15" s="7">
+        <v>1.4362916727687098</v>
+      </c>
+      <c r="G15" s="7">
+        <v>1.5836537648983082</v>
+      </c>
       <c r="I15">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.9069237317362473</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>1.0605900214686215</v>
       </c>
       <c r="J15">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.8176238723574909</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1.4456978880009448</v>
       </c>
       <c r="K15">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.58481962633573925</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1.1094924179231018</v>
       </c>
       <c r="Q15">
-        <v>0.27182050816483427</v>
+        <v>1.8969500821504357</v>
       </c>
       <c r="R15">
-        <v>0.58597495398797783</v>
+        <v>1.2613620731693187</v>
       </c>
       <c r="S15">
-        <v>0.27016164147456445</v>
+        <v>1.4718076548657861</v>
       </c>
     </row>
     <row r="16" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B16" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="6" cm="1">
+        <f t="array" ref="C16">_xll.AFBI.ALLOCATION.MAXIMUM(portfolio, sigma)</f>
+        <v>1.5788205116095568</v>
+      </c>
       <c r="I16">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.36728955937028152</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>1.5271304793380702</v>
       </c>
       <c r="J16">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.55020606012164874</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1.7195895350647197</v>
       </c>
       <c r="K16">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.67354109822452679</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1.4161407517637508</v>
       </c>
       <c r="Q16">
-        <v>0.28059889646508418</v>
+        <v>1.2178584677796958</v>
       </c>
       <c r="R16">
-        <v>0.45397435547944143</v>
+        <v>1.0457368707176511</v>
       </c>
       <c r="S16">
-        <v>0.33769334947986485</v>
-      </c>
-    </row>
-    <row r="17" spans="9:19" x14ac:dyDescent="0.25">
+        <v>1.4073504844857792</v>
+      </c>
+    </row>
+    <row r="17" spans="7:19" x14ac:dyDescent="0.25">
+      <c r="G17" s="3"/>
       <c r="I17">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.3447889129128604</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>1.7447826786545129</v>
       </c>
       <c r="J17">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.74104944347896284</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1.4039915704005259</v>
       </c>
       <c r="K17">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.53464981994445027</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1.1902683535629215</v>
       </c>
       <c r="Q17">
-        <v>0.8096649982640155</v>
+        <v>1.8053708137907278</v>
       </c>
       <c r="R17">
-        <v>0.62036392322361</v>
+        <v>1.5831177414364979</v>
       </c>
       <c r="S17">
-        <v>0.98032899332366574</v>
-      </c>
-    </row>
-    <row r="18" spans="9:19" x14ac:dyDescent="0.25">
+        <v>1.891053538016314</v>
+      </c>
+    </row>
+    <row r="18" spans="7:19" x14ac:dyDescent="0.25">
       <c r="I18">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.24048446667266976</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>1.8214512069779492</v>
       </c>
       <c r="J18">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.38428183090394774</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1.0984156059111094</v>
       </c>
       <c r="K18">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.64518272502373208</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1.4469808880911876</v>
       </c>
       <c r="Q18">
-        <v>0.5844503016940783</v>
+        <v>1.8691417890589197</v>
       </c>
       <c r="R18">
-        <v>0.41810702925768239</v>
+        <v>1.706983089981714</v>
       </c>
       <c r="S18">
-        <v>0.24749569043597108</v>
-      </c>
-    </row>
-    <row r="19" spans="9:19" x14ac:dyDescent="0.25">
+        <v>1.1029108665637288</v>
+      </c>
+    </row>
+    <row r="19" spans="7:19" x14ac:dyDescent="0.25">
       <c r="I19">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.38176857998012559</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>1.6042550675902518</v>
       </c>
       <c r="J19">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.47391353614926179</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1.0606142793272886</v>
       </c>
       <c r="K19">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.63767724774208501</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1.5261013256112386</v>
       </c>
       <c r="Q19">
-        <v>8.9364142300166649E-2</v>
+        <v>1.6304399711826241</v>
       </c>
       <c r="R19">
-        <v>0.18820347182044961</v>
+        <v>1.7320127005330175</v>
       </c>
       <c r="S19">
-        <v>0.54113251182930977</v>
-      </c>
-    </row>
-    <row r="20" spans="9:19" x14ac:dyDescent="0.25">
+        <v>1.0944561667368395</v>
+      </c>
+    </row>
+    <row r="20" spans="7:19" x14ac:dyDescent="0.25">
       <c r="I20">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.47670254528897815</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>1.9931231474732312</v>
       </c>
       <c r="J20">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.26000464291338099</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1.3151642461151303</v>
       </c>
       <c r="K20">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.38635730172279936</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1.6640339074395998</v>
       </c>
       <c r="Q20">
-        <v>0.47428766391466881</v>
+        <v>1.9210617726905115</v>
       </c>
       <c r="R20">
-        <v>0.68831669215467184</v>
+        <v>1.9378169377402177</v>
       </c>
       <c r="S20">
-        <v>0.17709079828185315</v>
-      </c>
-    </row>
-    <row r="21" spans="9:19" x14ac:dyDescent="0.25">
+        <v>1.2938579832855246</v>
+      </c>
+    </row>
+    <row r="21" spans="7:19" x14ac:dyDescent="0.25">
       <c r="I21">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.11584804220809763</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>1.0622486935038256</v>
       </c>
       <c r="J21">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.88582557640732595</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1.9176758605921682</v>
       </c>
       <c r="K21">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.78042107981291586</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1.8538937295562432</v>
       </c>
       <c r="Q21">
-        <v>0.82671117525781768</v>
+        <v>1.9669020224222367</v>
       </c>
       <c r="R21">
-        <v>0.93846464276956931</v>
+        <v>1.0653438308378402</v>
       </c>
       <c r="S21">
-        <v>9.737953602847127E-2</v>
+        <v>1.1982429441733133</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
portfolio constructor does cholesky decomposition now.
</commit_message>
<xml_diff>
--- a/excel/test.xlsx
+++ b/excel/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1009dev\source\repos\xlladdins\xll_allocation\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC8C5D5-98C1-4917-B12B-FC8BBD028823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF02E793-9D26-4E55-B15A-FC51D6972B3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C1522A91-786E-4C1B-8BA2-06271DEDE1ED}"/>
+    <workbookView xWindow="1470" yWindow="1470" windowWidth="21600" windowHeight="11385" xr2:uid="{C1522A91-786E-4C1B-8BA2-06271DEDE1ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -112,10 +112,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0E+00"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -304,7 +303,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -332,8 +331,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Input" xfId="1" builtinId="20"/>
@@ -652,9 +650,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{810AF907-DAD0-4E4A-8C49-374FAAA0C7DB}">
   <dimension ref="B1:W21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -695,27 +691,27 @@
       </c>
       <c r="I2">
         <f ca="1">1+RAND()</f>
-        <v>1.2515519641560882</v>
+        <v>1.6697070665880656</v>
       </c>
       <c r="J2">
         <f t="shared" ref="J2:K21" ca="1" si="2">1+RAND()</f>
-        <v>1.4509108495327752</v>
+        <v>1.3803531503958286</v>
       </c>
       <c r="K2">
         <f t="shared" ca="1" si="2"/>
-        <v>1.5881336184052435</v>
+        <v>1.6110942736483091</v>
       </c>
       <c r="M2" s="12" cm="1">
         <f t="array" aca="1" ref="M2:O5" ca="1">_xll.AFBI.COV(I2:K21)</f>
-        <v>1.4730727883134191</v>
+        <v>1.495532060075264</v>
       </c>
       <c r="N2" s="12">
         <f ca="1"/>
-        <v>1.4990664739415369</v>
+        <v>1.5650241295282969</v>
       </c>
       <c r="O2" s="12">
         <f ca="1"/>
-        <v>1.4539196142742736</v>
+        <v>1.5288504206854807</v>
       </c>
       <c r="Q2">
         <v>1.6724228739076512</v>
@@ -759,27 +755,27 @@
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I21" ca="1" si="4">1+RAND()</f>
-        <v>1.869393652474034</v>
+        <v>1.5037342266279281</v>
       </c>
       <c r="J3">
         <f t="shared" ca="1" si="2"/>
-        <v>1.5918178627603892</v>
+        <v>1.7373436169306917</v>
       </c>
       <c r="K3">
         <f t="shared" ca="1" si="2"/>
-        <v>1.0471462511659229</v>
+        <v>1.2975961444219668</v>
       </c>
       <c r="M3" s="13">
         <f ca="1"/>
-        <v>8.9416790656735579E-2</v>
+        <v>7.2547480052846058E-2</v>
       </c>
       <c r="N3" s="14">
         <f ca="1"/>
-        <v>-3.650252548914823E-2</v>
+        <v>1.1780985500611241E-2</v>
       </c>
       <c r="O3" s="15">
         <f ca="1"/>
-        <v>-3.1689484116773414E-2</v>
+        <v>-1.7433455292488187E-2</v>
       </c>
       <c r="Q3">
         <v>1.0999296210412119</v>
@@ -815,27 +811,27 @@
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="4"/>
-        <v>1.2371885053201277</v>
+        <v>1.5512128136176291</v>
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="2"/>
-        <v>1.9263740234804103</v>
+        <v>1.720430032198323</v>
       </c>
       <c r="K4">
         <f t="shared" ca="1" si="2"/>
-        <v>1.6985111057602478</v>
+        <v>1.765420873869036</v>
       </c>
       <c r="M4" s="16">
         <f ca="1"/>
-        <v>-3.650252548914823E-2</v>
+        <v>1.1780985500611241E-2</v>
       </c>
       <c r="N4" s="17">
         <f ca="1"/>
-        <v>6.859345119450877E-2</v>
+        <v>6.9169027384173631E-2</v>
       </c>
       <c r="O4" s="18">
         <f ca="1"/>
-        <v>-3.5239991090780798E-3</v>
+        <v>2.1876554522054281E-2</v>
       </c>
       <c r="Q4">
         <v>1.4390575770759571</v>
@@ -871,27 +867,27 @@
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="4"/>
-        <v>1.9234280844635099</v>
+        <v>1.2079107040277988</v>
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="2"/>
-        <v>1.3969846673469326</v>
+        <v>1.0175962734685629</v>
       </c>
       <c r="K5">
         <f t="shared" ca="1" si="2"/>
-        <v>1.379117033554961</v>
+        <v>1.8534535533217107</v>
       </c>
       <c r="M5" s="19">
         <f ca="1"/>
-        <v>-3.1689484116773414E-2</v>
+        <v>-1.7433455292488187E-2</v>
       </c>
       <c r="N5" s="12">
         <f ca="1"/>
-        <v>-3.5239991090780798E-3</v>
+        <v>2.1876554522054281E-2</v>
       </c>
       <c r="O5" s="20">
         <f ca="1"/>
-        <v>8.3255955836111895E-2</v>
+        <v>8.4064906001926065E-2</v>
       </c>
       <c r="Q5">
         <v>1.8696199837738985</v>
@@ -918,7 +914,7 @@
       </c>
       <c r="C6" s="4" cm="1">
         <f t="array" ref="C6">_xll.\AFBI.ALLOCATION(ER, Cov)</f>
-        <v>2326360968624</v>
+        <v>2971905099360</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>2</v>
@@ -928,15 +924,15 @@
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="4"/>
-        <v>1.4416692628071441</v>
+        <v>1.7578439292542836</v>
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="2"/>
-        <v>1.0997575655561631</v>
+        <v>1.7591086519777384</v>
       </c>
       <c r="K6">
         <f t="shared" ca="1" si="2"/>
-        <v>1.9269821794457807</v>
+        <v>1.7974642046024707</v>
       </c>
       <c r="Q6">
         <v>1.8349353619490156</v>
@@ -971,15 +967,15 @@
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="4"/>
-        <v>1.5113478059673049</v>
+        <v>1.1498980152720146</v>
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="2"/>
-        <v>1.5535048358394339</v>
+        <v>1.7824399956949404</v>
       </c>
       <c r="K7">
         <f t="shared" ca="1" si="2"/>
-        <v>1.2245806991157648</v>
+        <v>1.9353324457726333</v>
       </c>
       <c r="N7" t="b">
         <f ca="1">N3=M4</f>
@@ -1037,15 +1033,15 @@
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="4"/>
-        <v>1.6369871838548611</v>
+        <v>1.2170706209598379</v>
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="2"/>
-        <v>1.5813858740180105</v>
+        <v>1.5914529845077585</v>
       </c>
       <c r="K8">
         <f t="shared" ca="1" si="2"/>
-        <v>1.0608325647168277</v>
+        <v>1.6656251984445638</v>
       </c>
       <c r="O8" t="b">
         <f ca="1">O4=N5</f>
@@ -1072,15 +1068,15 @@
     <row r="9" spans="2:23" x14ac:dyDescent="0.25">
       <c r="I9">
         <f t="shared" ca="1" si="4"/>
-        <v>1.0616072202264912</v>
+        <v>1.5583654434799423</v>
       </c>
       <c r="J9">
         <f t="shared" ca="1" si="2"/>
-        <v>1.2992708257527261</v>
+        <v>1.1711455651899896</v>
       </c>
       <c r="K9">
         <f t="shared" ca="1" si="2"/>
-        <v>1.9840081535601546</v>
+        <v>1.3805577143121239</v>
       </c>
       <c r="Q9">
         <v>1.3278353737671185</v>
@@ -1100,24 +1096,24 @@
       <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="5">
-        <v>1.4</v>
+      <c r="C10" s="11">
+        <v>3</v>
       </c>
       <c r="D10" s="21">
         <f>SUMPRODUCT(C11:E11,ER)</f>
-        <v>1.4581487863039357</v>
+        <v>3.0000000000002025</v>
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="4"/>
-        <v>1.3897496236130147</v>
+        <v>1.9182089714034358</v>
       </c>
       <c r="J10">
         <f t="shared" ca="1" si="2"/>
-        <v>1.4714862893839884</v>
+        <v>1.7262793982046616</v>
       </c>
       <c r="K10">
         <f t="shared" ca="1" si="2"/>
-        <v>1.7400119807125765</v>
+        <v>1.339423586615851</v>
       </c>
       <c r="Q10">
         <v>1.2285720898044827</v>
@@ -1135,31 +1131,31 @@
       </c>
       <c r="C11" s="6" cm="1">
         <f t="array" ref="C11:G11">_xll.AFBI.ALLOCATION.MINIMIZE(portfolio, R_, 0)</f>
-        <v>2.7720340661606484E-2</v>
+        <v>15.939645981829932</v>
       </c>
       <c r="D11" s="6">
-        <v>0.25677700476083176</v>
+        <v>-0.17458916531414306</v>
       </c>
       <c r="E11" s="6">
-        <v>0.71550265457753737</v>
+        <v>-14.765056816515667</v>
       </c>
       <c r="F11" s="7">
-        <v>0.97016263566332517</v>
+        <v>-43.427694258375681</v>
       </c>
       <c r="G11" s="7">
-        <v>-0.6290006033436395</v>
+        <v>29.190311614649126</v>
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="4"/>
-        <v>1.343009468397915</v>
+        <v>1.1647515425514234</v>
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="2"/>
-        <v>1.7356064579320023</v>
+        <v>1.9022521495406306</v>
       </c>
       <c r="K11">
         <f t="shared" ca="1" si="2"/>
-        <v>1.413019290402127</v>
+        <v>1.521323194366377</v>
       </c>
       <c r="Q11">
         <v>1.3684795590972687</v>
@@ -1189,19 +1185,19 @@
       </c>
       <c r="C12" s="6" cm="1">
         <f t="array" ref="C12">_xll.AFBI.ALLOCATION.MINIMUM(portfolio, R_)</f>
-        <v>0.29926876045158723</v>
+        <v>6.6440379729176513</v>
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="4"/>
-        <v>1.1793482205886003</v>
+        <v>1.6574582389702828</v>
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="2"/>
-        <v>1.928901645530315</v>
+        <v>1.6966234253751162</v>
       </c>
       <c r="K12">
         <f t="shared" ca="1" si="2"/>
-        <v>1.5149579307556136</v>
+        <v>1.4444736686619573</v>
       </c>
       <c r="Q12">
         <v>1.2199462308238882</v>
@@ -1224,15 +1220,15 @@
     <row r="13" spans="2:23" x14ac:dyDescent="0.25">
       <c r="I13">
         <f t="shared" ca="1" si="4"/>
-        <v>1.7012777582817056</v>
+        <v>1.3412168712653785</v>
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="2"/>
-        <v>1.2742271485801546</v>
+        <v>1.4198702267659964</v>
       </c>
       <c r="K13">
         <f t="shared" ca="1" si="2"/>
-        <v>1.0249552587668149</v>
+        <v>1.0105535624711677</v>
       </c>
       <c r="Q13">
         <v>1.7151340649864826</v>
@@ -1253,23 +1249,23 @@
         <v>1</v>
       </c>
       <c r="C14" s="11">
-        <v>0.3</v>
-      </c>
-      <c r="D14" s="22">
-        <f>SUMPRODUCT(MMULT(ER,Cov),ER)</f>
-        <v>0.72856343914929411</v>
+        <v>10</v>
+      </c>
+      <c r="D14" s="21">
+        <f>SQRT(SUMPRODUCT(MMULT(weight,Cov),weight))</f>
+        <v>10.000000004201645</v>
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="4"/>
-        <v>1.1013157211111264</v>
+        <v>1.1627344712077221</v>
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="2"/>
-        <v>1.7099524477055468</v>
+        <v>1.3958635199819283</v>
       </c>
       <c r="K14">
         <f t="shared" ca="1" si="2"/>
-        <v>1.2692248451753936</v>
+        <v>1.9061523731092229</v>
       </c>
       <c r="Q14">
         <v>1.1151597871905503</v>
@@ -1287,31 +1283,31 @@
       </c>
       <c r="C15" s="6" cm="1">
         <f t="array" ref="C15:G15">_xll.AFBI.ALLOCATION.MAXIMIZE(portfolio, sigma, 0)</f>
-        <v>0.72521836666867401</v>
+        <v>23.823610052475608</v>
       </c>
       <c r="D15" s="6">
-        <v>0.21672360817836653</v>
+        <v>-0.39158416934868195</v>
       </c>
       <c r="E15" s="6">
-        <v>5.8058025152956189E-2</v>
+        <v>-22.432025883126929</v>
       </c>
       <c r="F15" s="7">
-        <v>1.4362916727687098</v>
+        <v>1.4881469506830507</v>
       </c>
       <c r="G15" s="7">
-        <v>1.5836537648983082</v>
+        <v>2.2756052233738444E-2</v>
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="4"/>
-        <v>1.0605900214686215</v>
+        <v>1.3860588692067117</v>
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="2"/>
-        <v>1.4456978880009448</v>
+        <v>1.8456217280388578</v>
       </c>
       <c r="K15">
         <f t="shared" ca="1" si="2"/>
-        <v>1.1094924179231018</v>
+        <v>1.678884487601195</v>
       </c>
       <c r="Q15">
         <v>1.8969500821504357</v>
@@ -1329,19 +1325,19 @@
       </c>
       <c r="C16" s="6" cm="1">
         <f t="array" ref="C16">_xll.AFBI.ALLOCATION.MAXIMUM(portfolio, sigma)</f>
-        <v>1.5788205116095568</v>
+        <v>3.763752175969119</v>
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="4"/>
-        <v>1.5271304793380702</v>
+        <v>1.8589504101690344</v>
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="2"/>
-        <v>1.7195895350647197</v>
+        <v>1.7437110799784437</v>
       </c>
       <c r="K16">
         <f t="shared" ca="1" si="2"/>
-        <v>1.4161407517637508</v>
+        <v>1.5952207512192476</v>
       </c>
       <c r="Q16">
         <v>1.2178584677796958</v>
@@ -1357,15 +1353,15 @@
       <c r="G17" s="3"/>
       <c r="I17">
         <f t="shared" ca="1" si="4"/>
-        <v>1.7447826786545129</v>
+        <v>1.9609228356458723</v>
       </c>
       <c r="J17">
         <f t="shared" ca="1" si="2"/>
-        <v>1.4039915704005259</v>
+        <v>1.5561282666423395</v>
       </c>
       <c r="K17">
         <f t="shared" ca="1" si="2"/>
-        <v>1.1902683535629215</v>
+        <v>1.0609465808332752</v>
       </c>
       <c r="Q17">
         <v>1.8053708137907278</v>
@@ -1380,15 +1376,15 @@
     <row r="18" spans="7:19" x14ac:dyDescent="0.25">
       <c r="I18">
         <f t="shared" ca="1" si="4"/>
-        <v>1.8214512069779492</v>
+        <v>1.0303281169774361</v>
       </c>
       <c r="J18">
         <f t="shared" ca="1" si="2"/>
-        <v>1.0984156059111094</v>
+        <v>1.353848035274374</v>
       </c>
       <c r="K18">
         <f t="shared" ca="1" si="2"/>
-        <v>1.4469808880911876</v>
+        <v>1.1043191762938696</v>
       </c>
       <c r="Q18">
         <v>1.8691417890589197</v>
@@ -1403,15 +1399,15 @@
     <row r="19" spans="7:19" x14ac:dyDescent="0.25">
       <c r="I19">
         <f t="shared" ca="1" si="4"/>
-        <v>1.6042550675902518</v>
+        <v>1.6505685893579696</v>
       </c>
       <c r="J19">
         <f t="shared" ca="1" si="2"/>
-        <v>1.0606142793272886</v>
+        <v>1.488121160731646</v>
       </c>
       <c r="K19">
         <f t="shared" ca="1" si="2"/>
-        <v>1.5261013256112386</v>
+        <v>1.3707095848128135</v>
       </c>
       <c r="Q19">
         <v>1.6304399711826241</v>
@@ -1426,15 +1422,15 @@
     <row r="20" spans="7:19" x14ac:dyDescent="0.25">
       <c r="I20">
         <f t="shared" ca="1" si="4"/>
-        <v>1.9931231474732312</v>
+        <v>1.5746944212359666</v>
       </c>
       <c r="J20">
         <f t="shared" ca="1" si="2"/>
-        <v>1.3151642461151303</v>
+        <v>1.9420724690409839</v>
       </c>
       <c r="K20">
         <f t="shared" ca="1" si="2"/>
-        <v>1.6640339074395998</v>
+        <v>1.9799054674818759</v>
       </c>
       <c r="Q20">
         <v>1.9210617726905115</v>
@@ -1449,15 +1445,15 @@
     <row r="21" spans="7:19" x14ac:dyDescent="0.25">
       <c r="I21">
         <f t="shared" ca="1" si="4"/>
-        <v>1.0622486935038256</v>
+        <v>1.5890050436865442</v>
       </c>
       <c r="J21">
         <f t="shared" ca="1" si="2"/>
-        <v>1.9176758605921682</v>
+        <v>1.0702208606271246</v>
       </c>
       <c r="K21">
         <f t="shared" ca="1" si="2"/>
-        <v>1.8538937295562432</v>
+        <v>1.2585515718499465</v>
       </c>
       <c r="Q21">
         <v>1.9669020224222367</v>

</xml_diff>